<commit_message>
PRGE week 7 update
</commit_message>
<xml_diff>
--- a/data/falo_rm.xlsx
+++ b/data/falo_rm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon/BrICC Clinic/BrICC Terms/Spring 2020/pilot_data_2020/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F6F960-C537-2D4F-9FA1-EC1190417319}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29468AC-71E7-D14F-A999-3FBD2A8697BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16260" xr2:uid="{319ED74C-C250-7347-91A7-75B74FF3BC61}"/>
+    <workbookView xWindow="34380" yWindow="3400" windowWidth="28040" windowHeight="16260" xr2:uid="{319ED74C-C250-7347-91A7-75B74FF3BC61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -411,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC198FF3-DBAF-924F-B22C-984517F50891}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -482,6 +482,35 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
PRGE and FALO week 8
</commit_message>
<xml_diff>
--- a/data/falo_rm.xlsx
+++ b/data/falo_rm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon/BrICC Clinic/BrICC Terms/Spring 2020/pilot_data_2020/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29468AC-71E7-D14F-A999-3FBD2A8697BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BDFE4FF-0165-9D4F-84D3-E242C09EA908}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34380" yWindow="3400" windowWidth="28040" windowHeight="16260" xr2:uid="{319ED74C-C250-7347-91A7-75B74FF3BC61}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" xr2:uid="{319ED74C-C250-7347-91A7-75B74FF3BC61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -411,15 +411,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC198FF3-DBAF-924F-B22C-984517F50891}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -448,12 +448,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
@@ -482,7 +482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
@@ -509,6 +509,35 @@
       </c>
       <c r="I4">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>